<commit_message>
feat: edit func changed to accept list with tuple
</commit_message>
<xml_diff>
--- a/excel_files/Empresas1.xlsx
+++ b/excel_files/Empresas1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Empresas" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
   <si>
     <t>DOMÍNIO SISTEMAS</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>ZARDUST</t>
+  </si>
+  <si>
+    <t>FUSCALDO ADMINISTRA</t>
   </si>
 </sst>
 </file>
@@ -825,8 +828,8 @@
   </sheetPr>
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,9 +863,8 @@
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="e">
-        <f>A3:A42FUSCALDO ADMINISTRA</f>
-        <v>#NAME?</v>
+      <c r="A3" t="s">
+        <v>81</v>
       </c>
       <c r="B3" s="12">
         <v>413</v>

</xml_diff>